<commit_message>
Updated Syntax Check to rename verified files in a using submission primary key
</commit_message>
<xml_diff>
--- a/AEF_files/11.syntax.failed/202405241221---AEF Guyana 2024 Revised 4 Final.syntax_checked.xlsx
+++ b/AEF_files/11.syntax.failed/202405241221---AEF Guyana 2024 Revised 4 Final.syntax_checked.xlsx
@@ -2448,17 +2448,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D325EA0-81F3-4144-913E-3E46B2D6CE25}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730B4CBF-6588-41DA-A413-8871750D837A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241F7104-F517-44C2-BF0B-E6EEC65F51C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFD4BB1-AE8C-4F1C-98C4-C72E7CB05488}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFA32DF4-4C13-4D4A-9BFD-1B9BD84EE2DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D83558F-8218-430E-83E9-87455B4A5F3D}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23718073-3614-4B3F-982B-3E3805D7C1B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15B7928-9E66-4877-84EB-EEB474211A2C}"/>
 </file>
</xml_diff>